<commit_message>
finished analysis with novelty, surprise, spark, motorfailure
</commit_message>
<xml_diff>
--- a/results_analysis/spark_motorFailure_02_hold2_novelty1.xlsx
+++ b/results_analysis/spark_motorFailure_02_hold2_novelty1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\MLTool_matlab\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720A3ED8-5E30-4A5D-9B58-4F4FA29108E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F1C4D0-AB90-46F4-9867-4C9E3A4209FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_best" sheetId="11" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="K_mean" sheetId="10" r:id="rId7"/>
     <sheet name="hp_best" sheetId="12" r:id="rId8"/>
     <sheet name="v1_v2_best" sheetId="13" r:id="rId9"/>
+    <sheet name="comp" sheetId="14" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="33">
   <si>
     <t>Sparsiciation Method</t>
   </si>
@@ -121,6 +122,18 @@
   <si>
     <t>v2</t>
   </si>
+  <si>
+    <t>Motor Failure DataSet 02 - Accuracy (best)</t>
+  </si>
+  <si>
+    <t>Motor Failure DataSet 02 - Accuracy (median)</t>
+  </si>
+  <si>
+    <t>Motor Failure DataSet 02 - Nprot (best)</t>
+  </si>
+  <si>
+    <t>Motor Failure DataSet 02 - Nprot (mean)</t>
+  </si>
 </sst>
 </file>
 
@@ -141,7 +154,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,12 +170,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -643,12 +650,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -769,6 +770,40 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1054,7 +1089,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,19 +1107,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
+      <c r="A1" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1153,7 +1188,7 @@
       <c r="J5" s="12">
         <v>0.67763157894736903</v>
       </c>
-      <c r="K5" s="43">
+      <c r="K5" s="41">
         <v>0.94078947368421095</v>
       </c>
     </row>
@@ -1282,7 +1317,7 @@
       <c r="J9" s="23">
         <v>0.93421052631579005</v>
       </c>
-      <c r="K9" s="42">
+      <c r="K9" s="40">
         <v>0.94736842105263197</v>
       </c>
     </row>
@@ -1390,16 +1425,16 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="29">
         <v>0.94736842105263197</v>
       </c>
       <c r="E13" s="23">
         <v>0.94736842105263197</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="23">
         <v>0.95394736842105299</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="23">
         <v>0.96052631578947401</v>
       </c>
       <c r="H13" s="23">
@@ -1411,7 +1446,7 @@
       <c r="J13" s="23">
         <v>0.88157894736842102</v>
       </c>
-      <c r="K13" s="42">
+      <c r="K13" s="40">
         <v>0.96052631578947401</v>
       </c>
     </row>
@@ -1423,13 +1458,13 @@
       <c r="D14" s="14">
         <v>0.94078947368421095</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="15">
         <v>1</v>
       </c>
       <c r="F14" s="15">
         <v>0.96052631578947401</v>
       </c>
-      <c r="G14" s="40">
+      <c r="G14" s="15">
         <v>0.95394736842105299</v>
       </c>
       <c r="H14" s="15">
@@ -1441,7 +1476,7 @@
       <c r="J14" s="15">
         <v>0.92763157894736903</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14" s="26">
         <v>0.97368421052631604</v>
       </c>
     </row>
@@ -1465,10 +1500,10 @@
       <c r="G15" s="15">
         <v>0.96710526315789502</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="15">
         <v>0.94736842105263197</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="15">
         <v>0.95394736842105299</v>
       </c>
       <c r="J15" s="15">
@@ -1977,12 +2012,1256 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0BA95D-B3FC-4D79-9A1A-0F5EE5F97F5E}">
+  <dimension ref="A1:W40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17:W17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="M1" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+    </row>
+    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="29">
+        <v>4.5999999999999902E-2</v>
+      </c>
+      <c r="E4" s="23">
+        <v>6.0000000000000097E-3</v>
+      </c>
+      <c r="F4" s="23">
+        <v>2.5999999999999902E-2</v>
+      </c>
+      <c r="G4" s="23">
+        <v>5.2999999999999901E-2</v>
+      </c>
+      <c r="H4" s="23">
+        <v>6.0000000000000097E-3</v>
+      </c>
+      <c r="I4" s="23">
+        <v>1.99999999999999E-2</v>
+      </c>
+      <c r="J4" s="23">
+        <v>-5.89999999999999E-2</v>
+      </c>
+      <c r="K4" s="40">
+        <v>2.6999999999999899E-2</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3">
+        <v>1</v>
+      </c>
+      <c r="P4" s="90">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="60">
+        <v>146</v>
+      </c>
+      <c r="R4" s="60">
+        <v>48</v>
+      </c>
+      <c r="S4" s="60">
+        <v>97</v>
+      </c>
+      <c r="T4" s="60">
+        <v>81</v>
+      </c>
+      <c r="U4" s="60">
+        <v>64</v>
+      </c>
+      <c r="V4" s="60">
+        <v>26</v>
+      </c>
+      <c r="W4" s="61">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="14">
+        <v>2.6999999999999899E-2</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0</v>
+      </c>
+      <c r="F5" s="15">
+        <v>4.6999999999999903E-2</v>
+      </c>
+      <c r="G5" s="15">
+        <v>-4.5999999999999999E-2</v>
+      </c>
+      <c r="H5" s="15">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="I5" s="15">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="J5" s="15">
+        <v>7.3000000000000106E-2</v>
+      </c>
+      <c r="K5" s="26">
+        <v>-2.5999999999999999E-2</v>
+      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="63">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="51">
+        <v>181</v>
+      </c>
+      <c r="R5" s="51">
+        <v>28</v>
+      </c>
+      <c r="S5" s="51">
+        <v>77</v>
+      </c>
+      <c r="T5" s="51">
+        <v>43</v>
+      </c>
+      <c r="U5" s="51">
+        <v>61</v>
+      </c>
+      <c r="V5" s="51">
+        <v>47</v>
+      </c>
+      <c r="W5" s="67">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14">
+        <v>2.5999999999999902E-2</v>
+      </c>
+      <c r="E6" s="15">
+        <v>4.6999999999999903E-2</v>
+      </c>
+      <c r="F6" s="15">
+        <v>3.8999999999999903E-2</v>
+      </c>
+      <c r="G6" s="15">
+        <v>6.0000000000000097E-3</v>
+      </c>
+      <c r="H6" s="15">
+        <v>6.0000000000000097E-3</v>
+      </c>
+      <c r="I6" s="15">
+        <v>1.99999999999999E-2</v>
+      </c>
+      <c r="J6" s="15">
+        <v>1.8999999999999899E-2</v>
+      </c>
+      <c r="K6" s="26">
+        <v>4.5999999999999902E-2</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="1">
+        <v>2</v>
+      </c>
+      <c r="O6" s="1">
+        <v>1</v>
+      </c>
+      <c r="P6" s="63">
+        <v>32</v>
+      </c>
+      <c r="Q6" s="51">
+        <v>83</v>
+      </c>
+      <c r="R6" s="51">
+        <v>63</v>
+      </c>
+      <c r="S6" s="51">
+        <v>86</v>
+      </c>
+      <c r="T6" s="51">
+        <v>95</v>
+      </c>
+      <c r="U6" s="51">
+        <v>123</v>
+      </c>
+      <c r="V6" s="51">
+        <v>93</v>
+      </c>
+      <c r="W6" s="67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="18">
+        <v>3.2999999999999897E-2</v>
+      </c>
+      <c r="E7" s="19">
+        <v>-6.6000000000000003E-2</v>
+      </c>
+      <c r="F7" s="19">
+        <v>2.5999999999999902E-2</v>
+      </c>
+      <c r="G7" s="19">
+        <v>-2.5999999999999999E-2</v>
+      </c>
+      <c r="H7" s="19">
+        <v>0</v>
+      </c>
+      <c r="I7" s="19">
+        <v>6.0000000000000097E-3</v>
+      </c>
+      <c r="J7" s="19">
+        <v>-7.0000000000000097E-3</v>
+      </c>
+      <c r="K7" s="27">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" s="64">
+        <v>57</v>
+      </c>
+      <c r="Q7" s="71">
+        <v>49</v>
+      </c>
+      <c r="R7" s="71">
+        <v>15</v>
+      </c>
+      <c r="S7" s="71">
+        <v>25</v>
+      </c>
+      <c r="T7" s="71">
+        <v>51</v>
+      </c>
+      <c r="U7" s="71">
+        <v>42</v>
+      </c>
+      <c r="V7" s="71">
+        <v>56</v>
+      </c>
+      <c r="W7" s="91">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="M9" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="74"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74"/>
+      <c r="Q9" s="74"/>
+      <c r="R9" s="74"/>
+      <c r="S9" s="74"/>
+      <c r="T9" s="74"/>
+      <c r="U9" s="74"/>
+      <c r="V9" s="74"/>
+      <c r="W9" s="74"/>
+    </row>
+    <row r="10" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
+    </row>
+    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="R11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="T11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="U11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="V11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="W11" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="29">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E12" s="23">
+        <v>-5.6000000000000098E-2</v>
+      </c>
+      <c r="F12" s="23">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="G12" s="23">
+        <v>-3.6999999999999998E-2</v>
+      </c>
+      <c r="H12" s="23">
+        <v>-2.9000000000000001E-2</v>
+      </c>
+      <c r="I12" s="23">
+        <v>-3.9E-2</v>
+      </c>
+      <c r="J12" s="23">
+        <v>-7.1999999999999995E-2</v>
+      </c>
+      <c r="K12" s="40">
+        <v>-3.7999999999999999E-2</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" s="3">
+        <v>1</v>
+      </c>
+      <c r="O12" s="3">
+        <v>1</v>
+      </c>
+      <c r="P12" s="84">
+        <v>50.8</v>
+      </c>
+      <c r="Q12" s="59">
+        <v>54.3</v>
+      </c>
+      <c r="R12" s="59">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="S12" s="59">
+        <v>47.5</v>
+      </c>
+      <c r="T12" s="59">
+        <v>55.2</v>
+      </c>
+      <c r="U12" s="59">
+        <v>43.1</v>
+      </c>
+      <c r="V12" s="59">
+        <v>11.7</v>
+      </c>
+      <c r="W12" s="85">
+        <v>55.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E13" s="15">
+        <v>-7.8E-2</v>
+      </c>
+      <c r="F13" s="15">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="G13" s="15">
+        <v>-8.6999999999999994E-2</v>
+      </c>
+      <c r="H13" s="15">
+        <v>2.4999999999999901E-2</v>
+      </c>
+      <c r="I13" s="15">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J13" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="K13" s="26">
+        <v>-3.6999999999999901E-2</v>
+      </c>
+      <c r="M13" s="4"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13" s="86">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="38">
+        <v>96.6</v>
+      </c>
+      <c r="R13" s="38">
+        <v>35</v>
+      </c>
+      <c r="S13" s="38">
+        <v>59.7</v>
+      </c>
+      <c r="T13" s="38">
+        <v>42.3</v>
+      </c>
+      <c r="U13" s="38">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="V13" s="38">
+        <v>17.7</v>
+      </c>
+      <c r="W13" s="87">
+        <v>52.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="E14" s="15">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="F14" s="15">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="G14" s="15">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H14" s="15">
+        <v>-2.1999999999999999E-2</v>
+      </c>
+      <c r="I14" s="15">
+        <v>-4.1000000000000002E-2</v>
+      </c>
+      <c r="J14" s="15">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="K14" s="26">
+        <v>-2.7E-2</v>
+      </c>
+      <c r="M14" s="4"/>
+      <c r="N14" s="1">
+        <v>2</v>
+      </c>
+      <c r="O14" s="1">
+        <v>1</v>
+      </c>
+      <c r="P14" s="86">
+        <v>39.4</v>
+      </c>
+      <c r="Q14" s="38">
+        <v>58.3</v>
+      </c>
+      <c r="R14" s="38">
+        <v>52.2</v>
+      </c>
+      <c r="S14" s="38">
+        <v>71.5</v>
+      </c>
+      <c r="T14" s="38">
+        <v>54.7</v>
+      </c>
+      <c r="U14" s="38">
+        <v>31</v>
+      </c>
+      <c r="V14" s="38">
+        <v>22.9</v>
+      </c>
+      <c r="W14" s="87">
+        <v>64.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="18">
+        <v>2.4E-2</v>
+      </c>
+      <c r="E15" s="19">
+        <v>-0.125</v>
+      </c>
+      <c r="F15" s="19">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G15" s="19">
+        <v>-7.8E-2</v>
+      </c>
+      <c r="H15" s="19">
+        <v>5.09999999999999E-2</v>
+      </c>
+      <c r="I15" s="19">
+        <v>-6.0000000000000097E-3</v>
+      </c>
+      <c r="J15" s="19">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="K15" s="27">
+        <v>-0.01</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P15" s="88">
+        <v>26.5</v>
+      </c>
+      <c r="Q15" s="70">
+        <v>54.9</v>
+      </c>
+      <c r="R15" s="70">
+        <v>28.5</v>
+      </c>
+      <c r="S15" s="70">
+        <v>56.1</v>
+      </c>
+      <c r="T15" s="70">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="U15" s="70">
+        <v>26.2</v>
+      </c>
+      <c r="V15" s="70">
+        <v>22.5</v>
+      </c>
+      <c r="W15" s="89">
+        <v>66.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="28"/>
+    </row>
+    <row r="17" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="74"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="74"/>
+      <c r="K17" s="74"/>
+      <c r="M17" s="80"/>
+      <c r="N17" s="80"/>
+      <c r="O17" s="80"/>
+      <c r="P17" s="80"/>
+      <c r="Q17" s="80"/>
+      <c r="R17" s="80"/>
+      <c r="S17" s="80"/>
+      <c r="T17" s="80"/>
+      <c r="U17" s="80"/>
+      <c r="V17" s="80"/>
+      <c r="W17" s="80"/>
+    </row>
+    <row r="18" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="81"/>
+      <c r="N18" s="81"/>
+      <c r="O18" s="81"/>
+      <c r="P18" s="81"/>
+      <c r="Q18" s="81"/>
+      <c r="R18" s="81"/>
+      <c r="S18" s="81"/>
+      <c r="T18" s="81"/>
+      <c r="U18" s="81"/>
+      <c r="V18" s="81"/>
+      <c r="W18" s="81"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="29">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E19" s="23">
+        <v>-5.1999999999999998E-2</v>
+      </c>
+      <c r="F19" s="23">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G19" s="23">
+        <v>-9.0000000000000097E-3</v>
+      </c>
+      <c r="H19" s="23">
+        <v>-0.01</v>
+      </c>
+      <c r="I19" s="23">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J19" s="23">
+        <v>-6.6000000000000003E-2</v>
+      </c>
+      <c r="K19" s="40">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="M19" s="81"/>
+      <c r="N19" s="81"/>
+      <c r="O19" s="81"/>
+      <c r="P19" s="82"/>
+      <c r="Q19" s="82"/>
+      <c r="R19" s="82"/>
+      <c r="S19" s="82"/>
+      <c r="T19" s="82"/>
+      <c r="U19" s="82"/>
+      <c r="V19" s="82"/>
+      <c r="W19" s="82"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="14">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E20" s="15">
+        <v>-0.105</v>
+      </c>
+      <c r="F20" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="G20" s="15">
+        <v>-8.8999999999999996E-2</v>
+      </c>
+      <c r="H20" s="15">
+        <v>4.6999999999999903E-2</v>
+      </c>
+      <c r="I20" s="15">
+        <v>2.39999999999999E-2</v>
+      </c>
+      <c r="J20" s="15">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K20" s="26">
+        <v>-2.6999999999999899E-2</v>
+      </c>
+      <c r="M20" s="81"/>
+      <c r="N20" s="81"/>
+      <c r="O20" s="81"/>
+      <c r="P20" s="82"/>
+      <c r="Q20" s="82"/>
+      <c r="R20" s="82"/>
+      <c r="S20" s="82"/>
+      <c r="T20" s="82"/>
+      <c r="U20" s="82"/>
+      <c r="V20" s="82"/>
+      <c r="W20" s="82"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="14">
+        <v>9.0000000000000097E-3</v>
+      </c>
+      <c r="E21" s="15">
+        <v>0.04</v>
+      </c>
+      <c r="F21" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="G21" s="15">
+        <v>7.0000000000000097E-3</v>
+      </c>
+      <c r="H21" s="15">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="I21" s="15">
+        <v>6.0000000000000097E-3</v>
+      </c>
+      <c r="J21" s="15">
+        <v>-1.9E-2</v>
+      </c>
+      <c r="K21" s="26">
+        <v>-0.02</v>
+      </c>
+      <c r="M21" s="81"/>
+      <c r="N21" s="81"/>
+      <c r="O21" s="81"/>
+      <c r="P21" s="82"/>
+      <c r="Q21" s="82"/>
+      <c r="R21" s="82"/>
+      <c r="S21" s="82"/>
+      <c r="T21" s="82"/>
+      <c r="U21" s="82"/>
+      <c r="V21" s="82"/>
+      <c r="W21" s="82"/>
+    </row>
+    <row r="22" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="18">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E22" s="19">
+        <v>-0.109</v>
+      </c>
+      <c r="F22" s="19">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="G22" s="19">
+        <v>-8.8999999999999996E-2</v>
+      </c>
+      <c r="H22" s="19">
+        <v>5.89999999999999E-2</v>
+      </c>
+      <c r="I22" s="19">
+        <v>9.9999999999998996E-3</v>
+      </c>
+      <c r="J22" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="K22" s="27">
+        <v>-0.01</v>
+      </c>
+      <c r="M22" s="81"/>
+      <c r="N22" s="81"/>
+      <c r="O22" s="81"/>
+      <c r="P22" s="82"/>
+      <c r="Q22" s="82"/>
+      <c r="R22" s="82"/>
+      <c r="S22" s="82"/>
+      <c r="T22" s="82"/>
+      <c r="U22" s="82"/>
+      <c r="V22" s="82"/>
+      <c r="W22" s="82"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="M23" s="83"/>
+      <c r="N23" s="83"/>
+      <c r="O23" s="83"/>
+      <c r="P23" s="83"/>
+      <c r="Q23" s="83"/>
+      <c r="R23" s="83"/>
+      <c r="S23" s="83"/>
+      <c r="T23" s="83"/>
+      <c r="U23" s="83"/>
+      <c r="V23" s="83"/>
+      <c r="W23" s="83"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="M24" s="83"/>
+      <c r="N24" s="83"/>
+      <c r="O24" s="83"/>
+      <c r="P24" s="83"/>
+      <c r="Q24" s="83"/>
+      <c r="R24" s="83"/>
+      <c r="S24" s="83"/>
+      <c r="T24" s="83"/>
+      <c r="U24" s="83"/>
+      <c r="V24" s="83"/>
+      <c r="W24" s="83"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+    </row>
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M9:W9"/>
+    <mergeCell ref="M17:W17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2000,19 +3279,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2318,7 +3597,7 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="29">
         <v>0.91842105263157903</v>
       </c>
       <c r="E13" s="23">
@@ -2333,13 +3612,13 @@
       <c r="H13" s="23">
         <v>0.86842105263157898</v>
       </c>
-      <c r="I13" s="24">
+      <c r="I13" s="23">
         <v>0.84210526315789502</v>
       </c>
       <c r="J13" s="23">
         <v>0.78881578947368403</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K13" s="40">
         <v>0.85065789473684195</v>
       </c>
     </row>
@@ -2357,13 +3636,13 @@
       <c r="F14" s="15">
         <v>0.91578947368421104</v>
       </c>
-      <c r="G14" s="40">
+      <c r="G14" s="15">
         <v>0.91184210526315801</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="15">
         <v>0.93815789473684197</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="15">
         <v>0.93421052631578905</v>
       </c>
       <c r="J14" s="15">
@@ -2910,7 +4189,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="D13" sqref="D13:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2928,19 +4207,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3246,7 +4525,7 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="15">
         <v>0.92434210526315796</v>
       </c>
       <c r="E13" s="15">
@@ -3255,19 +4534,19 @@
       <c r="F13" s="15">
         <v>0.92105263157894701</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="15">
         <v>0.88157894736842102</v>
       </c>
       <c r="H13" s="15">
         <v>0.88815789473684204</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="15">
         <v>0.88815789473684204</v>
       </c>
       <c r="J13" s="15">
         <v>0.79276315789473695</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="15">
         <v>0.90460526315789502</v>
       </c>
     </row>
@@ -3285,19 +4564,19 @@
       <c r="F14" s="15">
         <v>0.91118421052631604</v>
       </c>
-      <c r="G14" s="40">
+      <c r="G14" s="15">
         <v>0.91118421052631604</v>
       </c>
       <c r="H14" s="15">
         <v>0.96052631578947401</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="15">
         <v>0.9375</v>
       </c>
       <c r="J14" s="15">
         <v>0.80921052631579005</v>
       </c>
-      <c r="K14" s="16">
+      <c r="K14" s="15">
         <v>0.93421052631579005</v>
       </c>
     </row>
@@ -3680,7 +4959,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3698,19 +4977,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4016,7 +5295,7 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="38">
         <v>116</v>
       </c>
       <c r="E13" s="38">
@@ -4025,19 +5304,19 @@
       <c r="F13" s="38">
         <v>116</v>
       </c>
-      <c r="G13" s="39">
+      <c r="G13" s="38">
         <v>164</v>
       </c>
       <c r="H13" s="38">
         <v>154</v>
       </c>
-      <c r="I13" s="39">
+      <c r="I13" s="38">
         <v>140</v>
       </c>
       <c r="J13" s="38">
         <v>100</v>
       </c>
-      <c r="K13" s="39">
+      <c r="K13" s="38">
         <v>139</v>
       </c>
     </row>
@@ -4055,19 +5334,19 @@
       <c r="F14" s="38">
         <v>102</v>
       </c>
-      <c r="G14" s="41">
+      <c r="G14" s="38">
         <v>122</v>
       </c>
       <c r="H14" s="38">
         <v>115</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="38">
         <v>135</v>
       </c>
       <c r="J14" s="38">
         <v>104</v>
       </c>
-      <c r="K14" s="39">
+      <c r="K14" s="38">
         <v>104</v>
       </c>
     </row>
@@ -4468,19 +5747,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4786,7 +6065,7 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="38">
         <v>115.8</v>
       </c>
       <c r="E13" s="38">
@@ -4795,19 +6074,19 @@
       <c r="F13" s="38">
         <v>131.80000000000001</v>
       </c>
-      <c r="G13" s="39">
+      <c r="G13" s="38">
         <v>114.2</v>
       </c>
       <c r="H13" s="38">
         <v>125.2</v>
       </c>
-      <c r="I13" s="39">
+      <c r="I13" s="38">
         <v>114.8</v>
       </c>
       <c r="J13" s="38">
         <v>71.400000000000006</v>
       </c>
-      <c r="K13" s="39">
+      <c r="K13" s="38">
         <v>123.6</v>
       </c>
     </row>
@@ -4825,19 +6104,19 @@
       <c r="F14" s="38">
         <v>103.3</v>
       </c>
-      <c r="G14" s="41">
+      <c r="G14" s="38">
         <v>105.6</v>
       </c>
       <c r="H14" s="38">
         <v>110.6</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="38">
         <v>100.1</v>
       </c>
       <c r="J14" s="38">
         <v>74.599999999999994</v>
       </c>
-      <c r="K14" s="39">
+      <c r="K14" s="38">
         <v>110.6</v>
       </c>
     </row>
@@ -5238,19 +6517,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5556,7 +6835,7 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="38">
         <v>1</v>
       </c>
       <c r="E13" s="38">
@@ -5565,19 +6844,19 @@
       <c r="F13" s="38">
         <v>1</v>
       </c>
-      <c r="G13" s="39">
+      <c r="G13" s="38">
         <v>1</v>
       </c>
       <c r="H13" s="38">
         <v>1</v>
       </c>
-      <c r="I13" s="39">
+      <c r="I13" s="38">
         <v>1</v>
       </c>
       <c r="J13" s="38">
         <v>1</v>
       </c>
-      <c r="K13" s="39">
+      <c r="K13" s="38">
         <v>1</v>
       </c>
     </row>
@@ -5595,19 +6874,19 @@
       <c r="F14" s="38">
         <v>2</v>
       </c>
-      <c r="G14" s="41">
+      <c r="G14" s="38">
         <v>3</v>
       </c>
       <c r="H14" s="38">
         <v>7</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="38">
         <v>10</v>
       </c>
       <c r="J14" s="38">
         <v>2</v>
       </c>
-      <c r="K14" s="39">
+      <c r="K14" s="38">
         <v>6</v>
       </c>
     </row>
@@ -5990,7 +7269,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D13" sqref="D13:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6008,19 +7287,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6326,7 +7605,7 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="38">
         <v>1</v>
       </c>
       <c r="E13" s="38">
@@ -6335,19 +7614,19 @@
       <c r="F13" s="38">
         <v>1</v>
       </c>
-      <c r="G13" s="39">
+      <c r="G13" s="38">
         <v>1</v>
       </c>
       <c r="H13" s="38">
         <v>1</v>
       </c>
-      <c r="I13" s="39">
+      <c r="I13" s="38">
         <v>1</v>
       </c>
       <c r="J13" s="38">
         <v>1</v>
       </c>
-      <c r="K13" s="39">
+      <c r="K13" s="38">
         <v>1</v>
       </c>
     </row>
@@ -6365,19 +7644,19 @@
       <c r="F14" s="38">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G14" s="41">
+      <c r="G14" s="38">
         <v>4.2</v>
       </c>
       <c r="H14" s="38">
         <v>5.6</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="38">
         <v>6.1</v>
       </c>
       <c r="J14" s="38">
         <v>3.2</v>
       </c>
-      <c r="K14" s="39">
+      <c r="K14" s="38">
         <v>3.5</v>
       </c>
     </row>
@@ -6782,24 +8061,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6809,29 +8088,29 @@
       <c r="E3" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="77" t="s">
+      <c r="F3" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
       <c r="I3" s="36" t="s">
         <v>15</v>
       </c>
       <c r="J3" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="78" t="s">
+      <c r="K3" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="79"/>
-      <c r="M3" s="78" t="s">
+      <c r="L3" s="77"/>
+      <c r="M3" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="79"/>
-      <c r="O3" s="78" t="s">
+      <c r="N3" s="77"/>
+      <c r="O3" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="80"/>
+      <c r="P3" s="78"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -6840,46 +8119,46 @@
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="I4" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="49" t="s">
+      <c r="J4" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="49" t="s">
+      <c r="K4" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="49" t="s">
+      <c r="L4" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="49" t="s">
+      <c r="M4" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="N4" s="49" t="s">
+      <c r="N4" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="49" t="s">
+      <c r="O4" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="50" t="s">
+      <c r="P4" s="48" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6890,82 +8169,82 @@
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="45">
-        <v>1</v>
-      </c>
-      <c r="D5" s="74">
+      <c r="C5" s="43">
+        <v>1</v>
+      </c>
+      <c r="D5" s="72">
         <v>6.25E-2</v>
       </c>
-      <c r="E5" s="61">
+      <c r="E5" s="59">
         <v>0.5</v>
       </c>
-      <c r="F5" s="62">
-        <v>1</v>
-      </c>
-      <c r="G5" s="62">
-        <v>1</v>
-      </c>
-      <c r="H5" s="62">
+      <c r="F5" s="60">
+        <v>1</v>
+      </c>
+      <c r="G5" s="60">
+        <v>1</v>
+      </c>
+      <c r="H5" s="60">
         <v>3</v>
       </c>
-      <c r="I5" s="62">
+      <c r="I5" s="60">
         <v>128</v>
       </c>
-      <c r="J5" s="62">
+      <c r="J5" s="60">
         <v>2</v>
       </c>
-      <c r="K5" s="62">
+      <c r="K5" s="60">
         <v>3</v>
       </c>
-      <c r="L5" s="62">
+      <c r="L5" s="60">
         <v>4</v>
       </c>
-      <c r="M5" s="57">
+      <c r="M5" s="55">
         <v>3.125E-2</v>
       </c>
-      <c r="N5" s="60">
+      <c r="N5" s="58">
         <v>0.05</v>
       </c>
-      <c r="O5" s="62">
+      <c r="O5" s="60">
         <v>2</v>
       </c>
-      <c r="P5" s="63">
+      <c r="P5" s="61">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="65">
+      <c r="D6" s="63">
         <v>4</v>
       </c>
-      <c r="E6" s="56">
+      <c r="E6" s="54">
         <v>3.90625E-3</v>
       </c>
-      <c r="F6" s="53">
+      <c r="F6" s="51">
         <v>2</v>
       </c>
-      <c r="G6" s="54">
+      <c r="G6" s="52">
         <v>0.25</v>
       </c>
-      <c r="H6" s="53">
+      <c r="H6" s="51">
         <v>3</v>
       </c>
-      <c r="I6" s="54">
+      <c r="I6" s="52">
         <v>0.25</v>
       </c>
-      <c r="J6" s="55">
+      <c r="J6" s="53">
         <v>6.25E-2</v>
       </c>
       <c r="K6" s="38">
         <v>2.6</v>
       </c>
-      <c r="L6" s="55">
+      <c r="L6" s="53">
         <v>6.25E-2</v>
       </c>
-      <c r="M6" s="56">
+      <c r="M6" s="54">
         <v>3.90625E-3</v>
       </c>
       <c r="N6" s="15">
@@ -6983,10 +8262,10 @@
       <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="C7" s="46">
-        <v>1</v>
-      </c>
-      <c r="D7" s="65">
+      <c r="C7" s="44">
+        <v>1</v>
+      </c>
+      <c r="D7" s="63">
         <v>8</v>
       </c>
       <c r="E7" s="38">
@@ -6995,71 +8274,71 @@
       <c r="F7" s="38">
         <v>0.5</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="51">
         <v>8</v>
       </c>
-      <c r="H7" s="53">
+      <c r="H7" s="51">
         <v>3</v>
       </c>
-      <c r="I7" s="54">
+      <c r="I7" s="52">
         <v>0.25</v>
       </c>
-      <c r="J7" s="56">
+      <c r="J7" s="54">
         <v>3.125E-2</v>
       </c>
       <c r="K7" s="38">
         <v>0.4</v>
       </c>
-      <c r="L7" s="53">
+      <c r="L7" s="51">
         <v>16</v>
       </c>
-      <c r="M7" s="56">
+      <c r="M7" s="54">
         <v>3.90625E-3</v>
       </c>
       <c r="N7" s="15">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="O7" s="56">
+      <c r="O7" s="54">
         <v>7.8125E-3</v>
       </c>
-      <c r="P7" s="68">
+      <c r="P7" s="66">
         <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="65">
+      <c r="D8" s="63">
         <v>2</v>
       </c>
-      <c r="E8" s="56">
+      <c r="E8" s="54">
         <v>1.953125E-3</v>
       </c>
-      <c r="F8" s="53">
+      <c r="F8" s="51">
         <v>2</v>
       </c>
-      <c r="G8" s="53">
+      <c r="G8" s="51">
         <v>4</v>
       </c>
-      <c r="H8" s="53">
+      <c r="H8" s="51">
         <v>2</v>
       </c>
       <c r="I8" s="15">
         <v>0.125</v>
       </c>
-      <c r="J8" s="56">
+      <c r="J8" s="54">
         <v>3.125E-2</v>
       </c>
-      <c r="K8" s="53">
+      <c r="K8" s="51">
         <v>2</v>
       </c>
-      <c r="L8" s="53">
+      <c r="L8" s="51">
         <v>32</v>
       </c>
-      <c r="M8" s="56">
+      <c r="M8" s="54">
         <v>1.5625E-2</v>
       </c>
       <c r="N8" s="15">
@@ -7068,7 +8347,7 @@
       <c r="O8" s="38">
         <v>0.5</v>
       </c>
-      <c r="P8" s="68">
+      <c r="P8" s="66">
         <v>0.25</v>
       </c>
     </row>
@@ -7079,91 +8358,91 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="45">
-        <v>1</v>
-      </c>
-      <c r="D9" s="64">
+      <c r="C9" s="43">
+        <v>1</v>
+      </c>
+      <c r="D9" s="62">
         <v>6.25E-2</v>
       </c>
       <c r="E9" s="38">
         <v>0.5</v>
       </c>
-      <c r="F9" s="53">
+      <c r="F9" s="51">
         <v>4</v>
       </c>
-      <c r="G9" s="55">
+      <c r="G9" s="53">
         <v>6.25E-2</v>
       </c>
-      <c r="H9" s="53">
-        <v>1</v>
-      </c>
-      <c r="I9" s="53">
+      <c r="H9" s="51">
+        <v>1</v>
+      </c>
+      <c r="I9" s="51">
         <v>8</v>
       </c>
-      <c r="J9" s="56">
+      <c r="J9" s="54">
         <v>3.125E-2</v>
       </c>
       <c r="K9" s="38">
         <v>2.4</v>
       </c>
-      <c r="L9" s="53">
+      <c r="L9" s="51">
         <v>1024</v>
       </c>
-      <c r="M9" s="56">
+      <c r="M9" s="54">
         <v>7.8125E-3</v>
       </c>
       <c r="N9" s="15">
         <v>1E-3</v>
       </c>
-      <c r="O9" s="56">
+      <c r="O9" s="54">
         <v>3.90625E-3</v>
       </c>
-      <c r="P9" s="67">
+      <c r="P9" s="65">
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="62">
         <v>6.25E-2</v>
       </c>
-      <c r="E10" s="55">
+      <c r="E10" s="53">
         <v>6.25E-2</v>
       </c>
-      <c r="F10" s="53">
+      <c r="F10" s="51">
         <v>2</v>
       </c>
-      <c r="G10" s="53">
+      <c r="G10" s="51">
         <v>2</v>
       </c>
       <c r="H10" s="38">
         <v>0.6</v>
       </c>
-      <c r="I10" s="55">
+      <c r="I10" s="53">
         <v>6.25E-2</v>
       </c>
-      <c r="J10" s="56">
+      <c r="J10" s="54">
         <v>3.90625E-3</v>
       </c>
       <c r="K10" s="38">
         <v>2.8</v>
       </c>
-      <c r="L10" s="53">
-        <v>1</v>
-      </c>
-      <c r="M10" s="56">
+      <c r="L10" s="51">
+        <v>1</v>
+      </c>
+      <c r="M10" s="54">
         <v>3.125E-2</v>
       </c>
       <c r="N10" s="38">
         <v>0.1</v>
       </c>
-      <c r="O10" s="53">
+      <c r="O10" s="51">
         <v>8</v>
       </c>
-      <c r="P10" s="68">
+      <c r="P10" s="66">
         <v>0.25</v>
       </c>
     </row>
@@ -7172,16 +8451,16 @@
       <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="46">
-        <v>1</v>
-      </c>
-      <c r="D11" s="65">
+      <c r="C11" s="44">
+        <v>1</v>
+      </c>
+      <c r="D11" s="63">
         <v>1</v>
       </c>
       <c r="E11" s="38">
         <v>0.5</v>
       </c>
-      <c r="F11" s="55">
+      <c r="F11" s="53">
         <v>6.25E-2</v>
       </c>
       <c r="G11" s="15">
@@ -7190,41 +8469,41 @@
       <c r="H11" s="38">
         <v>0.6</v>
       </c>
-      <c r="I11" s="53">
+      <c r="I11" s="51">
         <v>32</v>
       </c>
-      <c r="J11" s="53">
+      <c r="J11" s="51">
         <v>2</v>
       </c>
       <c r="K11" s="38">
         <v>2.6</v>
       </c>
-      <c r="L11" s="53">
+      <c r="L11" s="51">
         <v>256</v>
       </c>
-      <c r="M11" s="55">
+      <c r="M11" s="53">
         <v>6.25E-2</v>
       </c>
       <c r="N11" s="15">
         <v>1E-3</v>
       </c>
-      <c r="O11" s="56">
+      <c r="O11" s="54">
         <v>3.90625E-3</v>
       </c>
-      <c r="P11" s="58">
+      <c r="P11" s="56">
         <v>3.125E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="65">
+      <c r="D12" s="63">
         <v>4</v>
       </c>
-      <c r="E12" s="55">
+      <c r="E12" s="53">
         <v>6.25E-2</v>
       </c>
       <c r="F12" s="15">
@@ -7236,28 +8515,28 @@
       <c r="H12" s="38">
         <v>0.8</v>
       </c>
-      <c r="I12" s="55">
+      <c r="I12" s="53">
         <v>6.25E-2</v>
       </c>
-      <c r="J12" s="56">
+      <c r="J12" s="54">
         <v>3.90625E-3</v>
       </c>
-      <c r="K12" s="53">
-        <v>1</v>
-      </c>
-      <c r="L12" s="53">
+      <c r="K12" s="51">
+        <v>1</v>
+      </c>
+      <c r="L12" s="51">
         <v>256</v>
       </c>
-      <c r="M12" s="56">
+      <c r="M12" s="54">
         <v>3.90625E-3</v>
       </c>
       <c r="N12" s="15">
         <v>0.01</v>
       </c>
-      <c r="O12" s="55">
+      <c r="O12" s="53">
         <v>6.25E-2</v>
       </c>
-      <c r="P12" s="67">
+      <c r="P12" s="65">
         <v>6.25E-2</v>
       </c>
     </row>
@@ -7268,88 +8547,88 @@
       <c r="B13" s="3">
         <v>1</v>
       </c>
-      <c r="C13" s="45">
-        <v>1</v>
-      </c>
-      <c r="D13" s="65">
+      <c r="C13" s="43">
+        <v>1</v>
+      </c>
+      <c r="D13" s="63">
         <v>64</v>
       </c>
-      <c r="E13" s="53">
+      <c r="E13" s="51">
         <v>4</v>
       </c>
       <c r="F13" s="15">
         <v>0.125</v>
       </c>
-      <c r="G13" s="53">
+      <c r="G13" s="51">
         <v>4</v>
       </c>
       <c r="H13" s="38">
         <v>0.6</v>
       </c>
-      <c r="I13" s="53">
+      <c r="I13" s="51">
         <v>256</v>
       </c>
-      <c r="J13" s="53">
+      <c r="J13" s="51">
         <v>1</v>
       </c>
       <c r="K13" s="38">
         <v>2.4</v>
       </c>
-      <c r="L13" s="53">
+      <c r="L13" s="51">
         <v>0.5</v>
       </c>
-      <c r="M13" s="55">
+      <c r="M13" s="53">
         <v>3.125E-2</v>
       </c>
       <c r="N13" s="15">
         <v>-7.8125E-3</v>
       </c>
-      <c r="O13" s="56">
+      <c r="O13" s="54">
         <v>3.125E-2</v>
       </c>
-      <c r="P13" s="69">
+      <c r="P13" s="67">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="65">
-        <v>1</v>
-      </c>
-      <c r="E14" s="55">
+      <c r="D14" s="63">
+        <v>1</v>
+      </c>
+      <c r="E14" s="53">
         <v>1.5625E-2</v>
       </c>
-      <c r="F14" s="53">
+      <c r="F14" s="51">
         <v>4</v>
       </c>
-      <c r="G14" s="55">
+      <c r="G14" s="53">
         <v>3.125E-2</v>
       </c>
-      <c r="H14" s="53">
-        <v>1</v>
-      </c>
-      <c r="I14" s="53">
+      <c r="H14" s="51">
+        <v>1</v>
+      </c>
+      <c r="I14" s="51">
         <v>128</v>
       </c>
-      <c r="J14" s="56">
+      <c r="J14" s="54">
         <v>1.953125E-3</v>
       </c>
       <c r="K14" s="38">
         <v>0.6</v>
       </c>
-      <c r="L14" s="54">
+      <c r="L14" s="52">
         <v>0.25</v>
       </c>
       <c r="M14" s="15">
         <v>0.125</v>
       </c>
-      <c r="N14" s="53">
+      <c r="N14" s="51">
         <v>-2</v>
       </c>
-      <c r="O14" s="53">
+      <c r="O14" s="51">
         <v>2</v>
       </c>
       <c r="P14" s="26">
@@ -7361,92 +8640,92 @@
       <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="C15" s="46">
-        <v>1</v>
-      </c>
-      <c r="D15" s="65">
+      <c r="C15" s="44">
+        <v>1</v>
+      </c>
+      <c r="D15" s="63">
         <v>0.5</v>
       </c>
-      <c r="E15" s="53">
-        <v>1</v>
-      </c>
-      <c r="F15" s="53">
+      <c r="E15" s="51">
+        <v>1</v>
+      </c>
+      <c r="F15" s="51">
         <v>64</v>
       </c>
-      <c r="G15" s="53">
+      <c r="G15" s="51">
         <v>2</v>
       </c>
-      <c r="H15" s="53">
+      <c r="H15" s="51">
         <v>3</v>
       </c>
-      <c r="I15" s="53">
+      <c r="I15" s="51">
         <v>4</v>
       </c>
-      <c r="J15" s="53">
+      <c r="J15" s="51">
         <v>1</v>
       </c>
       <c r="K15" s="38">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L15" s="53">
-        <v>1</v>
-      </c>
-      <c r="M15" s="55">
+      <c r="L15" s="51">
+        <v>1</v>
+      </c>
+      <c r="M15" s="53">
         <v>1.5625E-2</v>
       </c>
-      <c r="N15" s="54">
+      <c r="N15" s="52">
         <v>1.5625E-2</v>
       </c>
-      <c r="O15" s="53">
+      <c r="O15" s="51">
         <v>32</v>
       </c>
-      <c r="P15" s="69">
+      <c r="P15" s="67">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="64">
+      <c r="D16" s="62">
         <v>1.5625E-2</v>
       </c>
-      <c r="E16" s="53">
+      <c r="E16" s="51">
         <v>2</v>
       </c>
-      <c r="F16" s="55">
+      <c r="F16" s="53">
         <v>6.25E-2</v>
       </c>
-      <c r="G16" s="53">
+      <c r="G16" s="51">
         <v>512</v>
       </c>
       <c r="H16" s="38">
         <v>2.4</v>
       </c>
-      <c r="I16" s="55">
+      <c r="I16" s="53">
         <v>1.953125E-3</v>
       </c>
-      <c r="J16" s="56">
+      <c r="J16" s="54">
         <v>9.765625E-4</v>
       </c>
-      <c r="K16" s="53">
+      <c r="K16" s="51">
         <v>2.4</v>
       </c>
-      <c r="L16" s="55">
+      <c r="L16" s="53">
         <v>9.765625E-4</v>
       </c>
-      <c r="M16" s="56">
+      <c r="M16" s="54">
         <v>6.25E-2</v>
       </c>
       <c r="N16" s="38">
         <v>6.25E-2</v>
       </c>
-      <c r="O16" s="54">
+      <c r="O16" s="52">
         <v>6.25E-2</v>
       </c>
-      <c r="P16" s="67">
+      <c r="P16" s="65">
         <v>6.25E-2</v>
       </c>
     </row>
@@ -7457,88 +8736,88 @@
       <c r="B17" s="1">
         <v>1</v>
       </c>
-      <c r="C17" s="46">
-        <v>1</v>
-      </c>
-      <c r="D17" s="64">
+      <c r="C17" s="44">
+        <v>1</v>
+      </c>
+      <c r="D17" s="62">
         <v>6.25E-2</v>
       </c>
-      <c r="E17" s="53">
+      <c r="E17" s="51">
         <v>4</v>
       </c>
       <c r="F17" s="15">
         <v>0.125</v>
       </c>
-      <c r="G17" s="53">
+      <c r="G17" s="51">
         <v>4</v>
       </c>
       <c r="H17" s="38">
         <v>2.4</v>
       </c>
-      <c r="I17" s="53">
+      <c r="I17" s="51">
         <v>32</v>
       </c>
       <c r="J17" s="38">
         <v>0.5</v>
       </c>
-      <c r="K17" s="53">
-        <v>1</v>
-      </c>
-      <c r="L17" s="53">
+      <c r="K17" s="51">
+        <v>1</v>
+      </c>
+      <c r="L17" s="51">
         <v>512</v>
       </c>
-      <c r="M17" s="56">
+      <c r="M17" s="54">
         <v>3.90625E-3</v>
       </c>
       <c r="N17" s="38">
         <v>0.1</v>
       </c>
-      <c r="O17" s="53">
-        <v>1</v>
-      </c>
-      <c r="P17" s="69">
+      <c r="O17" s="51">
+        <v>1</v>
+      </c>
+      <c r="P17" s="67">
         <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="64">
+      <c r="D18" s="62">
         <v>6.25E-2</v>
       </c>
-      <c r="E18" s="56">
+      <c r="E18" s="54">
         <v>3.90625E-3</v>
       </c>
-      <c r="F18" s="53">
+      <c r="F18" s="51">
         <v>2</v>
       </c>
-      <c r="G18" s="53">
+      <c r="G18" s="51">
         <v>2</v>
       </c>
-      <c r="H18" s="53">
+      <c r="H18" s="51">
         <v>3</v>
       </c>
-      <c r="I18" s="53">
+      <c r="I18" s="51">
         <v>8</v>
       </c>
-      <c r="J18" s="56">
+      <c r="J18" s="54">
         <v>7.8125E-3</v>
       </c>
-      <c r="K18" s="53">
+      <c r="K18" s="51">
         <v>2</v>
       </c>
-      <c r="L18" s="53">
+      <c r="L18" s="51">
         <v>1024</v>
       </c>
-      <c r="M18" s="56">
+      <c r="M18" s="54">
         <v>3.90625E-3</v>
       </c>
       <c r="N18" s="38">
         <v>0.1</v>
       </c>
-      <c r="O18" s="53">
+      <c r="O18" s="51">
         <v>4</v>
       </c>
       <c r="P18" s="26">
@@ -7550,19 +8829,19 @@
       <c r="B19" s="1">
         <v>2</v>
       </c>
-      <c r="C19" s="46">
-        <v>1</v>
-      </c>
-      <c r="D19" s="64">
+      <c r="C19" s="44">
+        <v>1</v>
+      </c>
+      <c r="D19" s="62">
         <v>6.25E-2</v>
       </c>
       <c r="E19" s="38">
         <v>0.5</v>
       </c>
-      <c r="F19" s="53">
+      <c r="F19" s="51">
         <v>2</v>
       </c>
-      <c r="G19" s="53">
+      <c r="G19" s="51">
         <v>8</v>
       </c>
       <c r="H19" s="38">
@@ -7571,71 +8850,71 @@
       <c r="I19" s="15">
         <v>0.125</v>
       </c>
-      <c r="J19" s="55">
+      <c r="J19" s="53">
         <v>6.25E-2</v>
       </c>
       <c r="K19" s="38">
         <v>0.4</v>
       </c>
-      <c r="L19" s="53">
+      <c r="L19" s="51">
         <v>256</v>
       </c>
-      <c r="M19" s="56">
+      <c r="M19" s="54">
         <v>3.125E-2</v>
       </c>
       <c r="N19" s="15">
         <v>1E-3</v>
       </c>
-      <c r="O19" s="53">
-        <v>1</v>
-      </c>
-      <c r="P19" s="68">
+      <c r="O19" s="51">
+        <v>1</v>
+      </c>
+      <c r="P19" s="66">
         <v>0.25</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="47" t="s">
+      <c r="C20" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="66">
+      <c r="D20" s="64">
         <v>8</v>
       </c>
-      <c r="E20" s="59">
+      <c r="E20" s="57">
         <v>1.5625E-2</v>
       </c>
-      <c r="F20" s="73">
+      <c r="F20" s="71">
         <v>4</v>
       </c>
-      <c r="G20" s="71">
+      <c r="G20" s="69">
         <v>0.25</v>
       </c>
-      <c r="H20" s="72">
+      <c r="H20" s="70">
         <v>2.8</v>
       </c>
-      <c r="I20" s="59">
+      <c r="I20" s="57">
         <v>3.125E-2</v>
       </c>
-      <c r="J20" s="59">
+      <c r="J20" s="57">
         <v>3.125E-2</v>
       </c>
-      <c r="K20" s="72">
+      <c r="K20" s="70">
         <v>0.4</v>
       </c>
-      <c r="L20" s="73">
+      <c r="L20" s="71">
         <v>256</v>
       </c>
-      <c r="M20" s="59">
+      <c r="M20" s="57">
         <v>3.125E-2</v>
       </c>
       <c r="N20" s="19">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="O20" s="70">
+      <c r="O20" s="68">
         <v>6.25E-2</v>
       </c>
-      <c r="P20" s="75">
+      <c r="P20" s="73">
         <v>6.25E-2</v>
       </c>
     </row>
@@ -7897,7 +9176,7 @@
   <dimension ref="A1:S53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7917,61 +9196,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
+      <c r="A1" s="74" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="81" t="s">
+      <c r="D3" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="79"/>
-      <c r="F3" s="78" t="s">
+      <c r="E3" s="77"/>
+      <c r="F3" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="79"/>
-      <c r="H3" s="78" t="s">
+      <c r="G3" s="77"/>
+      <c r="H3" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="79"/>
-      <c r="J3" s="78" t="s">
+      <c r="I3" s="77"/>
+      <c r="J3" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="79"/>
-      <c r="L3" s="78" t="s">
+      <c r="K3" s="77"/>
+      <c r="L3" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="79"/>
-      <c r="N3" s="78" t="s">
+      <c r="M3" s="77"/>
+      <c r="N3" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="79"/>
-      <c r="P3" s="78" t="s">
+      <c r="O3" s="77"/>
+      <c r="P3" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="78" t="s">
+      <c r="Q3" s="77"/>
+      <c r="R3" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="80"/>
+      <c r="S3" s="78"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -7983,52 +9262,52 @@
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="44" t="s">
+      <c r="G4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="44" t="s">
+      <c r="H4" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="44" t="s">
+      <c r="I4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="44" t="s">
+      <c r="J4" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="44" t="s">
+      <c r="K4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="44" t="s">
+      <c r="L4" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="44" t="s">
+      <c r="M4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="44" t="s">
+      <c r="N4" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="44" t="s">
+      <c r="O4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="44" t="s">
+      <c r="P4" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="44" t="s">
+      <c r="Q4" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="R4" s="44" t="s">
+      <c r="R4" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="S4" s="44" t="s">
+      <c r="S4" s="42" t="s">
         <v>28</v>
       </c>
     </row>
@@ -8042,52 +9321,52 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="52">
+      <c r="D5" s="50">
         <v>1.953125E-3</v>
       </c>
-      <c r="E5" s="51">
+      <c r="E5" s="49">
         <v>1024.001</v>
       </c>
-      <c r="F5" s="52">
+      <c r="F5" s="50">
         <v>1.5625E-2</v>
       </c>
-      <c r="G5" s="51">
+      <c r="G5" s="49">
         <v>1024.001</v>
       </c>
-      <c r="H5" s="52">
+      <c r="H5" s="50">
         <v>7.8125E-3</v>
       </c>
-      <c r="I5" s="51">
+      <c r="I5" s="49">
         <v>1024.001</v>
       </c>
       <c r="J5" s="12">
         <v>1.953125E-3</v>
       </c>
-      <c r="K5" s="51">
+      <c r="K5" s="49">
         <v>1024.001</v>
       </c>
       <c r="L5" s="12">
         <v>1.953125E-3</v>
       </c>
-      <c r="M5" s="51">
+      <c r="M5" s="49">
         <v>1024.001</v>
       </c>
       <c r="N5" s="12">
         <v>-0.125</v>
       </c>
-      <c r="O5" s="51">
+      <c r="O5" s="49">
         <v>1024.001</v>
       </c>
-      <c r="P5" s="52">
+      <c r="P5" s="50">
         <v>1.953125E-3</v>
       </c>
-      <c r="Q5" s="51">
+      <c r="Q5" s="49">
         <v>1024.001</v>
       </c>
-      <c r="R5" s="52">
+      <c r="R5" s="50">
         <v>1.953125E-3</v>
       </c>
-      <c r="S5" s="51">
+      <c r="S5" s="49">
         <v>1024.001</v>
       </c>
     </row>
@@ -8096,52 +9375,52 @@
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="55">
+      <c r="D6" s="53">
         <v>3.90625E-3</v>
       </c>
-      <c r="E6" s="53">
+      <c r="E6" s="51">
         <v>1024.001</v>
       </c>
       <c r="F6" s="38">
         <v>1</v>
       </c>
-      <c r="G6" s="53">
+      <c r="G6" s="51">
         <v>1024.001</v>
       </c>
-      <c r="H6" s="54">
+      <c r="H6" s="52">
         <v>0.25</v>
       </c>
-      <c r="I6" s="53">
+      <c r="I6" s="51">
         <v>1024.001</v>
       </c>
       <c r="J6" s="15">
         <v>0.125</v>
       </c>
-      <c r="K6" s="53">
+      <c r="K6" s="51">
         <v>1024.001</v>
       </c>
-      <c r="L6" s="54">
+      <c r="L6" s="52">
         <v>0.25</v>
       </c>
-      <c r="M6" s="53">
+      <c r="M6" s="51">
         <v>1024.001</v>
       </c>
-      <c r="N6" s="53">
+      <c r="N6" s="51">
         <v>-8</v>
       </c>
-      <c r="O6" s="53">
+      <c r="O6" s="51">
         <v>1024.001</v>
       </c>
-      <c r="P6" s="55">
+      <c r="P6" s="53">
         <v>3.90625E-3</v>
       </c>
-      <c r="Q6" s="53">
+      <c r="Q6" s="51">
         <v>1024.001</v>
       </c>
       <c r="R6" s="38">
         <v>1</v>
       </c>
-      <c r="S6" s="53">
+      <c r="S6" s="51">
         <v>1024.001</v>
       </c>
     </row>
@@ -8153,52 +9432,52 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="55">
+      <c r="D7" s="53">
         <v>1.953125E-3</v>
       </c>
-      <c r="E7" s="53">
+      <c r="E7" s="51">
         <v>1024.001</v>
       </c>
-      <c r="F7" s="55">
+      <c r="F7" s="53">
         <v>6.25E-2</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="51">
         <v>1024.001</v>
       </c>
-      <c r="H7" s="55">
+      <c r="H7" s="53">
         <v>7.8125E-3</v>
       </c>
-      <c r="I7" s="53">
+      <c r="I7" s="51">
         <v>1024.001</v>
       </c>
-      <c r="J7" s="54">
+      <c r="J7" s="52">
         <v>0.25</v>
       </c>
-      <c r="K7" s="53">
+      <c r="K7" s="51">
         <v>1024.001</v>
       </c>
       <c r="L7" s="38">
         <v>1</v>
       </c>
-      <c r="M7" s="53">
+      <c r="M7" s="51">
         <v>1024.001</v>
       </c>
-      <c r="N7" s="55">
+      <c r="N7" s="53">
         <v>-1.5625E-2</v>
       </c>
-      <c r="O7" s="53">
+      <c r="O7" s="51">
         <v>1024.001</v>
       </c>
-      <c r="P7" s="55">
+      <c r="P7" s="53">
         <v>1.953125E-3</v>
       </c>
-      <c r="Q7" s="53">
+      <c r="Q7" s="51">
         <v>1024.001</v>
       </c>
-      <c r="R7" s="54">
+      <c r="R7" s="52">
         <v>0.25</v>
       </c>
-      <c r="S7" s="53">
+      <c r="S7" s="51">
         <v>1024.001</v>
       </c>
     </row>
@@ -8208,52 +9487,52 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="55">
+      <c r="D8" s="53">
         <v>3.90625E-3</v>
       </c>
-      <c r="E8" s="53">
+      <c r="E8" s="51">
         <v>1024.001</v>
       </c>
-      <c r="F8" s="54">
+      <c r="F8" s="52">
         <v>0.25</v>
       </c>
-      <c r="G8" s="53">
+      <c r="G8" s="51">
         <v>1024.001</v>
       </c>
-      <c r="H8" s="53">
+      <c r="H8" s="51">
         <v>64</v>
       </c>
-      <c r="I8" s="53">
+      <c r="I8" s="51">
         <v>1024.001</v>
       </c>
       <c r="J8" s="38">
         <v>0.5</v>
       </c>
-      <c r="K8" s="53">
+      <c r="K8" s="51">
         <v>1024.001</v>
       </c>
       <c r="L8" s="38">
         <v>0.5</v>
       </c>
-      <c r="M8" s="53">
+      <c r="M8" s="51">
         <v>1024.001</v>
       </c>
       <c r="N8" s="15">
         <v>-0.125</v>
       </c>
-      <c r="O8" s="53">
+      <c r="O8" s="51">
         <v>1024.001</v>
       </c>
-      <c r="P8" s="55">
+      <c r="P8" s="53">
         <v>1.953125E-3</v>
       </c>
-      <c r="Q8" s="53">
+      <c r="Q8" s="51">
         <v>1024.001</v>
       </c>
       <c r="R8" s="38">
         <v>1</v>
       </c>
-      <c r="S8" s="53">
+      <c r="S8" s="51">
         <v>1024.001</v>
       </c>
     </row>
@@ -8267,7 +9546,7 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="54">
+      <c r="D9" s="52">
         <v>0.99</v>
       </c>
       <c r="E9" s="15">
@@ -8279,13 +9558,13 @@
       <c r="G9" s="15">
         <v>0.99099999999999999</v>
       </c>
-      <c r="H9" s="54">
+      <c r="H9" s="52">
         <v>0.99</v>
       </c>
       <c r="I9" s="15">
         <v>0.99099999999999999</v>
       </c>
-      <c r="J9" s="54">
+      <c r="J9" s="52">
         <v>0.99</v>
       </c>
       <c r="K9" s="15">
@@ -8303,7 +9582,7 @@
       <c r="O9" s="38">
         <v>1</v>
       </c>
-      <c r="P9" s="54">
+      <c r="P9" s="52">
         <v>0.99</v>
       </c>
       <c r="Q9" s="15">
@@ -8321,7 +9600,7 @@
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="54">
+      <c r="D10" s="52">
         <v>0.99</v>
       </c>
       <c r="E10" s="15">
@@ -8333,7 +9612,7 @@
       <c r="G10" s="15">
         <v>0.99099999999999999</v>
       </c>
-      <c r="H10" s="54">
+      <c r="H10" s="52">
         <v>0.99</v>
       </c>
       <c r="I10" s="15">
@@ -8345,25 +9624,25 @@
       <c r="K10" s="15">
         <v>0.99099999999999999</v>
       </c>
-      <c r="L10" s="54">
+      <c r="L10" s="52">
         <v>0.01</v>
       </c>
       <c r="M10" s="15">
         <v>0.99099999999999999</v>
       </c>
-      <c r="N10" s="54">
+      <c r="N10" s="52">
         <v>0.99</v>
       </c>
       <c r="O10" s="38">
         <v>1</v>
       </c>
-      <c r="P10" s="54">
+      <c r="P10" s="52">
         <v>0.99</v>
       </c>
       <c r="Q10" s="15">
         <v>0.99099999999999999</v>
       </c>
-      <c r="R10" s="54">
+      <c r="R10" s="52">
         <v>0.01</v>
       </c>
       <c r="S10" s="15">
@@ -8378,31 +9657,31 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="54">
+      <c r="D11" s="52">
         <v>0.9</v>
       </c>
       <c r="E11" s="15">
         <v>0.99099999999999999</v>
       </c>
-      <c r="F11" s="54">
+      <c r="F11" s="52">
         <v>0.9</v>
       </c>
       <c r="G11" s="15">
         <v>0.99099999999999999</v>
       </c>
-      <c r="H11" s="54">
+      <c r="H11" s="52">
         <v>0.99</v>
       </c>
       <c r="I11" s="15">
         <v>0.99099999999999999</v>
       </c>
-      <c r="J11" s="54">
+      <c r="J11" s="52">
         <v>0.99</v>
       </c>
       <c r="K11" s="15">
         <v>0.99099999999999999</v>
       </c>
-      <c r="L11" s="54">
+      <c r="L11" s="52">
         <v>0.99</v>
       </c>
       <c r="M11" s="15">
@@ -8414,7 +9693,7 @@
       <c r="O11" s="38">
         <v>1</v>
       </c>
-      <c r="P11" s="54">
+      <c r="P11" s="52">
         <v>0.99</v>
       </c>
       <c r="Q11" s="15">
@@ -8433,19 +9712,19 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="54">
+      <c r="D12" s="52">
         <v>0.99</v>
       </c>
       <c r="E12" s="15">
         <v>0.99099999999999999</v>
       </c>
-      <c r="F12" s="54">
+      <c r="F12" s="52">
         <v>0.01</v>
       </c>
       <c r="G12" s="15">
         <v>0.99099999999999999</v>
       </c>
-      <c r="H12" s="54">
+      <c r="H12" s="52">
         <v>0.99</v>
       </c>
       <c r="I12" s="15">
@@ -8457,7 +9736,7 @@
       <c r="K12" s="15">
         <v>0.99099999999999999</v>
       </c>
-      <c r="L12" s="54">
+      <c r="L12" s="52">
         <v>0.01</v>
       </c>
       <c r="M12" s="15">
@@ -8469,7 +9748,7 @@
       <c r="O12" s="38">
         <v>1</v>
       </c>
-      <c r="P12" s="54">
+      <c r="P12" s="52">
         <v>0.99</v>
       </c>
       <c r="Q12" s="15">
@@ -8501,7 +9780,7 @@
       <c r="F13" s="15">
         <v>1.953125E-3</v>
       </c>
-      <c r="G13" s="55">
+      <c r="G13" s="53">
         <v>3.22265625E-2</v>
       </c>
       <c r="H13" s="15">
@@ -8522,13 +9801,13 @@
       <c r="M13" s="38">
         <v>1.0009765625</v>
       </c>
-      <c r="N13" s="54">
+      <c r="N13" s="52">
         <v>0.25</v>
       </c>
       <c r="O13" s="38">
         <v>1.0009765625</v>
       </c>
-      <c r="P13" s="55">
+      <c r="P13" s="53">
         <v>3.90625E-3</v>
       </c>
       <c r="Q13" s="38">
@@ -8546,16 +9825,16 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="55">
+      <c r="D14" s="53">
         <v>3.90625E-3</v>
       </c>
       <c r="E14" s="15">
         <v>4.8828125E-3</v>
       </c>
-      <c r="F14" s="54">
+      <c r="F14" s="52">
         <v>0.25</v>
       </c>
-      <c r="G14" s="55">
+      <c r="G14" s="53">
         <v>6.34765625E-2</v>
       </c>
       <c r="H14" s="15">
@@ -8564,19 +9843,19 @@
       <c r="I14" s="15">
         <v>4.8828125E-3</v>
       </c>
-      <c r="J14" s="55">
+      <c r="J14" s="53">
         <v>3.90625E-3</v>
       </c>
-      <c r="K14" s="54">
+      <c r="K14" s="52">
         <v>1.66015625E-2</v>
       </c>
-      <c r="L14" s="55">
+      <c r="L14" s="53">
         <v>3.125E-2</v>
       </c>
       <c r="M14" s="38">
         <v>1.0009765625</v>
       </c>
-      <c r="N14" s="53">
+      <c r="N14" s="51">
         <v>2</v>
       </c>
       <c r="O14" s="38">
@@ -8585,7 +9864,7 @@
       <c r="P14" s="15">
         <v>9.765625E-4</v>
       </c>
-      <c r="Q14" s="55">
+      <c r="Q14" s="53">
         <v>3.22265625E-2</v>
       </c>
       <c r="R14" s="15">
@@ -8603,13 +9882,13 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="55">
+      <c r="D15" s="53">
         <v>3.125E-2</v>
       </c>
       <c r="E15" s="38">
         <v>1.0009765625</v>
       </c>
-      <c r="F15" s="54">
+      <c r="F15" s="52">
         <v>7.8125E-3</v>
       </c>
       <c r="G15" s="38">
@@ -8618,13 +9897,13 @@
       <c r="H15" s="38">
         <v>0.5</v>
       </c>
-      <c r="I15" s="53">
+      <c r="I15" s="51">
         <v>1.0009765625</v>
       </c>
       <c r="J15" s="15">
         <v>1.953125E-3</v>
       </c>
-      <c r="K15" s="53">
+      <c r="K15" s="51">
         <v>1.0009765625</v>
       </c>
       <c r="L15" s="15">
@@ -8633,7 +9912,7 @@
       <c r="M15" s="38">
         <v>1.0009765625</v>
       </c>
-      <c r="N15" s="54">
+      <c r="N15" s="52">
         <v>1.5625E-2</v>
       </c>
       <c r="O15" s="38">
@@ -8642,10 +9921,10 @@
       <c r="P15" s="15">
         <v>9.765625E-4</v>
       </c>
-      <c r="Q15" s="54">
+      <c r="Q15" s="52">
         <v>0.5009765625</v>
       </c>
-      <c r="R15" s="55">
+      <c r="R15" s="53">
         <v>3.90625E-3</v>
       </c>
       <c r="S15" s="38">
@@ -8658,13 +9937,13 @@
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="54">
+      <c r="D16" s="52">
         <v>1.5625E-2</v>
       </c>
       <c r="E16" s="15">
         <v>1.953125E-3</v>
       </c>
-      <c r="F16" s="54">
+      <c r="F16" s="52">
         <v>7.8125E-3</v>
       </c>
       <c r="G16" s="38">
@@ -8673,13 +9952,13 @@
       <c r="H16" s="15">
         <v>0.125</v>
       </c>
-      <c r="I16" s="53">
+      <c r="I16" s="51">
         <v>1.0009765625</v>
       </c>
-      <c r="J16" s="55">
+      <c r="J16" s="53">
         <v>3.90625E-3</v>
       </c>
-      <c r="K16" s="53">
+      <c r="K16" s="51">
         <v>1.0009765625</v>
       </c>
       <c r="L16" s="15">
@@ -8688,7 +9967,7 @@
       <c r="M16" s="38">
         <v>1.0009765625</v>
       </c>
-      <c r="N16" s="54">
+      <c r="N16" s="52">
         <v>0.25</v>
       </c>
       <c r="O16" s="38">
@@ -8717,28 +9996,28 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="53">
+      <c r="D17" s="51">
         <v>16</v>
       </c>
-      <c r="E17" s="53">
+      <c r="E17" s="51">
         <v>1024.0009765625</v>
       </c>
-      <c r="F17" s="53">
+      <c r="F17" s="51">
         <v>16</v>
       </c>
-      <c r="G17" s="53">
+      <c r="G17" s="51">
         <v>256.0009765625</v>
       </c>
-      <c r="H17" s="55">
+      <c r="H17" s="53">
         <v>7.8125E-3</v>
       </c>
-      <c r="I17" s="53">
+      <c r="I17" s="51">
         <v>64.0009765625</v>
       </c>
-      <c r="J17" s="55">
+      <c r="J17" s="53">
         <v>1.5625E-2</v>
       </c>
-      <c r="K17" s="55">
+      <c r="K17" s="53">
         <v>6.34765625E-2</v>
       </c>
       <c r="L17" s="15">
@@ -8747,22 +10026,22 @@
       <c r="M17" s="38">
         <v>0.5009765625</v>
       </c>
-      <c r="N17" s="53">
+      <c r="N17" s="51">
         <v>-128</v>
       </c>
       <c r="O17" s="15">
         <v>-9.765625E-4</v>
       </c>
-      <c r="P17" s="55">
+      <c r="P17" s="53">
         <v>3.90625E-3</v>
       </c>
-      <c r="Q17" s="53">
+      <c r="Q17" s="51">
         <v>8.0009765625</v>
       </c>
-      <c r="R17" s="53">
+      <c r="R17" s="51">
         <v>8</v>
       </c>
-      <c r="S17" s="53">
+      <c r="S17" s="51">
         <v>128.0009765625</v>
       </c>
     </row>
@@ -8771,37 +10050,37 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="53">
+      <c r="D18" s="51">
         <v>16</v>
       </c>
-      <c r="E18" s="53">
+      <c r="E18" s="51">
         <v>128.0009765625</v>
       </c>
-      <c r="F18" s="55">
+      <c r="F18" s="53">
         <v>1.5625E-2</v>
       </c>
       <c r="G18" s="38">
         <v>0.5009765625</v>
       </c>
-      <c r="H18" s="55">
+      <c r="H18" s="53">
         <v>7.8125E-3</v>
       </c>
-      <c r="I18" s="53">
+      <c r="I18" s="51">
         <v>2.0009765625</v>
       </c>
-      <c r="J18" s="53">
-        <v>1</v>
-      </c>
-      <c r="K18" s="53">
+      <c r="J18" s="51">
+        <v>1</v>
+      </c>
+      <c r="K18" s="51">
         <v>256.0009765625</v>
       </c>
-      <c r="L18" s="55">
+      <c r="L18" s="53">
         <v>1.953125E-3</v>
       </c>
       <c r="M18" s="15">
         <v>0.1259765625</v>
       </c>
-      <c r="N18" s="55">
+      <c r="N18" s="53">
         <v>-64</v>
       </c>
       <c r="O18" s="15">
@@ -8810,13 +10089,13 @@
       <c r="P18" s="15">
         <v>9.765625E-4</v>
       </c>
-      <c r="Q18" s="53">
+      <c r="Q18" s="51">
         <v>32.0009765625</v>
       </c>
-      <c r="R18" s="55">
+      <c r="R18" s="53">
         <v>1.953125E-3</v>
       </c>
-      <c r="S18" s="53">
+      <c r="S18" s="51">
         <v>16.0009765625</v>
       </c>
     </row>
@@ -8828,49 +10107,49 @@
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="55">
+      <c r="D19" s="53">
         <v>6.25E-2</v>
       </c>
-      <c r="E19" s="53">
+      <c r="E19" s="51">
         <v>32.0009765625</v>
       </c>
-      <c r="F19" s="54">
+      <c r="F19" s="52">
         <v>0.25</v>
       </c>
-      <c r="G19" s="53">
+      <c r="G19" s="51">
         <v>64.0009765625</v>
       </c>
-      <c r="H19" s="55">
+      <c r="H19" s="53">
         <v>1.953125E-3</v>
       </c>
-      <c r="I19" s="55">
+      <c r="I19" s="53">
         <v>3.22265625E-2</v>
       </c>
-      <c r="J19" s="55">
+      <c r="J19" s="53">
         <v>3.125E-2</v>
       </c>
-      <c r="K19" s="53">
+      <c r="K19" s="51">
         <v>32.0009765625</v>
       </c>
-      <c r="L19" s="55">
+      <c r="L19" s="53">
         <v>1.5625E-2</v>
       </c>
-      <c r="M19" s="53">
+      <c r="M19" s="51">
         <v>16.0009765625</v>
       </c>
-      <c r="N19" s="54">
+      <c r="N19" s="52">
         <v>-0.25</v>
       </c>
-      <c r="O19" s="53">
+      <c r="O19" s="51">
         <v>32.0009765625</v>
       </c>
-      <c r="P19" s="55">
+      <c r="P19" s="53">
         <v>7.8125E-3</v>
       </c>
-      <c r="Q19" s="53">
+      <c r="Q19" s="51">
         <v>8.0009765625</v>
       </c>
-      <c r="R19" s="55">
+      <c r="R19" s="53">
         <v>3.125E-2</v>
       </c>
       <c r="S19" s="15">
@@ -8883,40 +10162,40 @@
       <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="55">
+      <c r="D20" s="53">
         <v>1.5625E-2</v>
       </c>
-      <c r="E20" s="53">
+      <c r="E20" s="51">
         <v>32.0009765625</v>
       </c>
-      <c r="F20" s="55">
+      <c r="F20" s="53">
         <v>1.953125E-3</v>
       </c>
-      <c r="G20" s="55">
+      <c r="G20" s="53">
         <v>4.8828125E-3</v>
       </c>
-      <c r="H20" s="55">
+      <c r="H20" s="53">
         <v>7.8125E-3</v>
       </c>
       <c r="I20" s="15">
         <v>0.5009765625</v>
       </c>
-      <c r="J20" s="55">
+      <c r="J20" s="53">
         <v>3.125E-2</v>
       </c>
-      <c r="K20" s="55">
+      <c r="K20" s="53">
         <v>6.34765625E-2</v>
       </c>
-      <c r="L20" s="55">
+      <c r="L20" s="53">
         <v>1.5625E-2</v>
       </c>
-      <c r="M20" s="53">
+      <c r="M20" s="51">
         <v>1.0009765625</v>
       </c>
-      <c r="N20" s="53">
+      <c r="N20" s="51">
         <v>4</v>
       </c>
-      <c r="O20" s="53">
+      <c r="O20" s="51">
         <v>8.0009765625</v>
       </c>
       <c r="P20" s="15">
@@ -8925,7 +10204,7 @@
       <c r="Q20" s="15">
         <v>0.5009765625</v>
       </c>
-      <c r="R20" s="55">
+      <c r="R20" s="53">
         <v>1.953125E-3</v>
       </c>
       <c r="S20" s="15">

</xml_diff>